<commit_message>
feat: data files and statistics
</commit_message>
<xml_diff>
--- a/data/05 Oct Dataset@Wast.xlsx
+++ b/data/05 Oct Dataset@Wast.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rksanjeev/Desktop/BJN/checked data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{384B79F2-6A93-E947-88BF-F0631B7F4827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F19195E-6714-AF45-9B60-CECCD5FDDD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1600" windowWidth="27640" windowHeight="16400" xr2:uid="{A39FA76E-84AC-0C42-ABE4-8893D704C7A0}"/>
+    <workbookView xWindow="3420" yWindow="3200" windowWidth="27640" windowHeight="16400" xr2:uid="{A39FA76E-84AC-0C42-ABE4-8893D704C7A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>